<commit_message>
update sql file and ER
</commit_message>
<xml_diff>
--- a/ER.xlsx
+++ b/ER.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mid\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mid\Desktop\web2-app\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="8436" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9096" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="ER図（概）" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="185">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="183">
   <si>
     <t>PK: PRIMARY KEY</t>
   </si>
@@ -966,14 +966,6 @@
   </si>
   <si>
     <t>Order</t>
-    <phoneticPr fontId="3"/>
-  </si>
-  <si>
-    <t>DamyPassword</t>
-    <phoneticPr fontId="3"/>
-  </si>
-  <si>
-    <t>UserId</t>
     <phoneticPr fontId="3"/>
   </si>
 </sst>
@@ -1095,7 +1087,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1107,9 +1099,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1117,6 +1106,12 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -4070,8 +4065,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:Q56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="122" zoomScaleNormal="122" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8:I8"/>
+    <sheetView tabSelected="1" zoomScale="122" zoomScaleNormal="122" workbookViewId="0">
+      <selection activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12"/>
@@ -4094,11 +4089,11 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:13">
-      <c r="B2" s="9" t="s">
+      <c r="B2" s="12" t="s">
         <v>182</v>
       </c>
-      <c r="C2" s="9"/>
-      <c r="D2" s="9"/>
+      <c r="C2" s="12"/>
+      <c r="D2" s="12"/>
     </row>
     <row r="3" spans="2:13">
       <c r="B3" s="5" t="s">
@@ -4141,18 +4136,18 @@
       </c>
     </row>
     <row r="8" spans="2:13">
-      <c r="G8" s="9" t="s">
+      <c r="G8" s="12" t="s">
         <v>156</v>
       </c>
-      <c r="H8" s="9"/>
-      <c r="I8" s="9"/>
+      <c r="H8" s="12"/>
+      <c r="I8" s="12"/>
     </row>
     <row r="9" spans="2:13">
-      <c r="B9" s="9" t="s">
+      <c r="B9" s="12" t="s">
         <v>165</v>
       </c>
-      <c r="C9" s="9"/>
-      <c r="D9" s="9"/>
+      <c r="C9" s="12"/>
+      <c r="D9" s="12"/>
       <c r="G9" s="5" t="s">
         <v>162</v>
       </c>
@@ -4162,6 +4157,9 @@
       <c r="I9" s="5" t="s">
         <v>160</v>
       </c>
+      <c r="K9" s="8"/>
+      <c r="L9" s="8"/>
+      <c r="M9" s="8"/>
     </row>
     <row r="10" spans="2:13">
       <c r="B10" s="5" t="s">
@@ -4180,6 +4178,9 @@
       <c r="I10" s="5" t="s">
         <v>161</v>
       </c>
+      <c r="K10" s="8"/>
+      <c r="L10" s="8"/>
+      <c r="M10" s="8"/>
     </row>
     <row r="11" spans="2:13">
       <c r="B11" s="5" t="s">
@@ -4198,10 +4199,9 @@
       <c r="I11" s="5" t="s">
         <v>163</v>
       </c>
-      <c r="K11" s="9" t="s">
-        <v>183</v>
-      </c>
-      <c r="L11" s="9"/>
+      <c r="K11" s="13"/>
+      <c r="L11" s="13"/>
+      <c r="M11" s="8"/>
     </row>
     <row r="12" spans="2:13">
       <c r="B12" s="5"/>
@@ -4214,10 +4214,9 @@
       <c r="G12" s="8"/>
       <c r="H12" s="8"/>
       <c r="I12" s="8"/>
-      <c r="K12" s="5"/>
-      <c r="L12" s="5" t="s">
-        <v>184</v>
-      </c>
+      <c r="K12" s="8"/>
+      <c r="L12" s="8"/>
+      <c r="M12" s="8"/>
     </row>
     <row r="13" spans="2:13">
       <c r="B13" s="5"/>
@@ -4227,29 +4226,33 @@
       <c r="D13" s="5" t="s">
         <v>168</v>
       </c>
-      <c r="K13" s="5"/>
-      <c r="L13" s="5" t="s">
-        <v>183</v>
-      </c>
+      <c r="K13" s="8"/>
+      <c r="L13" s="8"/>
+      <c r="M13" s="8"/>
+    </row>
+    <row r="14" spans="2:13">
+      <c r="K14" s="8"/>
+      <c r="L14" s="8"/>
+      <c r="M14" s="8"/>
     </row>
     <row r="16" spans="2:13">
-      <c r="G16" s="9" t="s">
+      <c r="G16" s="12" t="s">
         <v>68</v>
       </c>
-      <c r="H16" s="9"/>
-      <c r="I16" s="9"/>
-      <c r="K16" s="9" t="s">
+      <c r="H16" s="12"/>
+      <c r="I16" s="12"/>
+      <c r="K16" s="12" t="s">
         <v>80</v>
       </c>
-      <c r="L16" s="9"/>
-      <c r="M16" s="9"/>
+      <c r="L16" s="12"/>
+      <c r="M16" s="12"/>
     </row>
     <row r="17" spans="2:17">
-      <c r="B17" s="9" t="s">
+      <c r="B17" s="12" t="s">
         <v>129</v>
       </c>
-      <c r="C17" s="9"/>
-      <c r="D17" s="9"/>
+      <c r="C17" s="12"/>
+      <c r="D17" s="12"/>
       <c r="G17" s="5" t="s">
         <v>91</v>
       </c>
@@ -4311,11 +4314,11 @@
       <c r="I19" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="O19" s="9" t="s">
+      <c r="O19" s="12" t="s">
         <v>136</v>
       </c>
-      <c r="P19" s="9"/>
-      <c r="Q19" s="9"/>
+      <c r="P19" s="12"/>
+      <c r="Q19" s="12"/>
     </row>
     <row r="20" spans="2:17">
       <c r="B20" s="7"/>
@@ -4402,11 +4405,11 @@
       </c>
     </row>
     <row r="25" spans="2:17">
-      <c r="K25" s="9" t="s">
+      <c r="K25" s="12" t="s">
         <v>164</v>
       </c>
-      <c r="L25" s="9"/>
-      <c r="M25" s="9"/>
+      <c r="L25" s="12"/>
+      <c r="M25" s="12"/>
     </row>
     <row r="26" spans="2:17">
       <c r="K26" s="5" t="s">
@@ -4420,11 +4423,11 @@
       </c>
     </row>
     <row r="27" spans="2:17">
-      <c r="B27" s="9" t="s">
+      <c r="B27" s="12" t="s">
         <v>132</v>
       </c>
-      <c r="C27" s="9"/>
-      <c r="D27" s="9"/>
+      <c r="C27" s="12"/>
+      <c r="D27" s="12"/>
       <c r="K27" s="5" t="s">
         <v>44</v>
       </c>
@@ -4492,11 +4495,11 @@
       </c>
     </row>
     <row r="32" spans="2:17">
-      <c r="G32" s="9" t="s">
+      <c r="G32" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="H32" s="9"/>
-      <c r="I32" s="9"/>
+      <c r="H32" s="12"/>
+      <c r="I32" s="12"/>
       <c r="K32" s="5" t="s">
         <v>99</v>
       </c>
@@ -4544,11 +4547,11 @@
       <c r="I36" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="K36" s="9" t="s">
+      <c r="K36" s="12" t="s">
         <v>144</v>
       </c>
-      <c r="L36" s="9"/>
-      <c r="M36" s="9"/>
+      <c r="L36" s="12"/>
+      <c r="M36" s="12"/>
     </row>
     <row r="37" spans="2:13">
       <c r="G37" s="5"/>
@@ -4569,11 +4572,11 @@
       </c>
     </row>
     <row r="38" spans="2:13">
-      <c r="B38" s="10" t="s">
+      <c r="B38" s="9" t="s">
         <v>113</v>
       </c>
-      <c r="C38" s="11"/>
-      <c r="D38" s="12"/>
+      <c r="C38" s="10"/>
+      <c r="D38" s="11"/>
       <c r="G38" s="5"/>
       <c r="H38" s="5" t="s">
         <v>88</v>
@@ -4669,11 +4672,11 @@
       </c>
     </row>
     <row r="45" spans="2:13">
-      <c r="B45" s="10" t="s">
+      <c r="B45" s="9" t="s">
         <v>117</v>
       </c>
-      <c r="C45" s="11"/>
-      <c r="D45" s="12"/>
+      <c r="C45" s="10"/>
+      <c r="D45" s="11"/>
     </row>
     <row r="46" spans="2:13">
       <c r="B46" s="5" t="s">
@@ -4707,11 +4710,11 @@
       </c>
     </row>
     <row r="53" spans="2:4">
-      <c r="B53" s="10" t="s">
+      <c r="B53" s="9" t="s">
         <v>120</v>
       </c>
-      <c r="C53" s="11"/>
-      <c r="D53" s="12"/>
+      <c r="C53" s="10"/>
+      <c r="D53" s="11"/>
     </row>
     <row r="54" spans="2:4">
       <c r="B54" s="5" t="s">
@@ -4746,11 +4749,6 @@
     </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="B45:D45"/>
-    <mergeCell ref="B53:D53"/>
-    <mergeCell ref="B17:D17"/>
-    <mergeCell ref="B27:D27"/>
-    <mergeCell ref="B38:D38"/>
     <mergeCell ref="B2:D2"/>
     <mergeCell ref="O19:Q19"/>
     <mergeCell ref="K36:M36"/>
@@ -4761,6 +4759,11 @@
     <mergeCell ref="G8:I8"/>
     <mergeCell ref="B9:D9"/>
     <mergeCell ref="K11:L11"/>
+    <mergeCell ref="B45:D45"/>
+    <mergeCell ref="B53:D53"/>
+    <mergeCell ref="B17:D17"/>
+    <mergeCell ref="B27:D27"/>
+    <mergeCell ref="B38:D38"/>
   </mergeCells>
   <phoneticPr fontId="3"/>
   <dataValidations xWindow="260" yWindow="566" count="31">

</xml_diff>